<commit_message>
Working with date object.
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/diamondRule.xlsx
+++ b/src/main/resources/rules/diamondRule.xlsx
@@ -167,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -205,19 +205,6 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
-        <color indexed="8"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="hair">
         <color indexed="8"/>
@@ -231,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -270,13 +257,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -296,13 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -695,7 +679,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -737,7 +721,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -759,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -770,7 +754,7 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="41.21875" customWidth="1"/>
     <col min="8" max="8" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -861,7 +845,7 @@
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>

</xml_diff>

<commit_message>
date comparator is working
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/diamondRule.xlsx
+++ b/src/main/resources/rules/diamondRule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>RuleSet</t>
   </si>
@@ -51,9 +51,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>com.app.drools.api.model.Product</t>
-  </si>
-  <si>
     <t>quality</t>
   </si>
   <si>
@@ -106,6 +103,16 @@
   </si>
   <si>
     <t>purchasedDate</t>
+  </si>
+  <si>
+    <t>com.app.drools.api.model.Product,
+java.util.*,
+java.text.ParseException,
+java.text.SimpleDateFormat,
+java.util.Date</t>
+  </si>
+  <si>
+    <t>purchasedDate before("$param")</t>
   </si>
 </sst>
 </file>
@@ -743,19 +750,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="5" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="41.21875" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="36.44140625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" outlineLevel="1">
@@ -772,12 +779,12 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="2" spans="1:8" ht="38.1" customHeight="1" outlineLevel="1">
+    <row r="2" spans="1:8" ht="86.4" customHeight="1" outlineLevel="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -840,7 +847,7 @@
     </row>
     <row r="7" spans="1:8" outlineLevel="1">
       <c r="B7" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -855,22 +862,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" outlineLevel="1">
@@ -881,30 +888,30 @@
         <v>10</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" outlineLevel="1">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -919,13 +926,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -939,16 +946,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="17"/>
@@ -961,16 +968,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="E13" s="10">
         <v>100</v>
@@ -987,19 +994,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="10">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="7">
@@ -1011,16 +1018,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="E15" s="10">
         <v>100</v>

</xml_diff>

<commit_message>
RESt with drools working with GET
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/diamondRule.xlsx
+++ b/src/main/resources/rules/diamondRule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>RuleSet</t>
   </si>
@@ -99,20 +99,47 @@
     <t>Diamond#6</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>purchasedDate</t>
-  </si>
-  <si>
-    <t>com.app.drools.api.model.Product,
-java.util.*,
-java.text.ParseException,
-java.text.SimpleDateFormat,
-java.util.Date</t>
-  </si>
-  <si>
-    <t>purchasedDate before("$param")</t>
+    <t>Diamond#7</t>
+  </si>
+  <si>
+    <t>Diamond#8</t>
+  </si>
+  <si>
+    <t>Diamond#9</t>
+  </si>
+  <si>
+    <t>Diamond#10</t>
+  </si>
+  <si>
+    <t>Diamond#11</t>
+  </si>
+  <si>
+    <t>Diamond#12</t>
+  </si>
+  <si>
+    <t>Diamond#13</t>
+  </si>
+  <si>
+    <t>Diamond#14</t>
+  </si>
+  <si>
+    <t>Diamond#15</t>
+  </si>
+  <si>
+    <t>Diamond#16</t>
+  </si>
+  <si>
+    <t>Equal purchasedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purchasedDate </t>
+  </si>
+  <si>
+    <t>$productObject.getType()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.app.drools.api.model.Product
+</t>
   </si>
 </sst>
 </file>
@@ -261,9 +288,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -287,7 +311,10 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,7 +713,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -728,7 +755,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -748,19 +775,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" customWidth="1"/>
     <col min="3" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" style="19" customWidth="1"/>
     <col min="7" max="7" width="26.5546875" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -779,19 +806,19 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="2" spans="1:8" ht="86.4" customHeight="1" outlineLevel="1">
+    <row r="2" spans="1:8" ht="26.4" outlineLevel="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" outlineLevel="1">
       <c r="A3" s="1" t="s">
@@ -803,7 +830,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="19"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
@@ -815,7 +842,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -835,7 +862,7 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -859,7 +886,7 @@
     <row r="8" spans="1:8" ht="26.4" outlineLevel="1">
       <c r="A8" s="9"/>
       <c r="B8" s="12" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>11</v>
@@ -870,8 +897,8 @@
       <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>30</v>
+      <c r="F8" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>14</v>
@@ -896,8 +923,8 @@
       <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>28</v>
+      <c r="F9" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>6</v>
@@ -916,9 +943,9 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="17"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="7">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H10" s="14">
         <v>1</v>
@@ -934,11 +961,13 @@
       <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E11" s="10"/>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="7">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H11" s="14">
         <v>2</v>
@@ -954,13 +983,11 @@
       <c r="C12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="17"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="7">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H12" s="14">
         <v>3</v>
@@ -982,11 +1009,11 @@
       <c r="E13" s="10">
         <v>100</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>40645</v>
       </c>
       <c r="G13" s="7">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="H13" s="14">
         <v>4</v>
@@ -1000,17 +1027,17 @@
         <v>15</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="10">
-        <v>700</v>
-      </c>
-      <c r="F14" s="17"/>
+        <v>120</v>
+      </c>
+      <c r="F14" s="16"/>
       <c r="G14" s="7">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H14" s="14">
         <v>5</v>
@@ -1030,16 +1057,256 @@
         <v>17</v>
       </c>
       <c r="E15" s="10">
-        <v>100</v>
-      </c>
-      <c r="F15" s="24">
-        <v>42088</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F15" s="23"/>
       <c r="G15" s="7">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="H15" s="14">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="10">
+        <v>160</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="G16" s="7">
+        <v>7</v>
+      </c>
+      <c r="H16" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="10">
+        <v>180</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="7">
+        <v>8</v>
+      </c>
+      <c r="H17" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="10">
+        <v>200</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="7">
+        <v>9</v>
+      </c>
+      <c r="H18" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="10">
+        <v>220</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="7">
+        <v>10</v>
+      </c>
+      <c r="H19" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="10">
+        <v>240</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="7">
+        <v>11</v>
+      </c>
+      <c r="H20" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="10">
+        <v>260</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="7">
+        <v>12</v>
+      </c>
+      <c r="H21" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="10">
+        <v>280</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="7">
+        <v>13</v>
+      </c>
+      <c r="H22" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="10">
+        <v>300</v>
+      </c>
+      <c r="F23" s="23">
+        <v>40490</v>
+      </c>
+      <c r="G23" s="7">
+        <v>14</v>
+      </c>
+      <c r="H23" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="10">
+        <v>320</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="7">
+        <v>15</v>
+      </c>
+      <c r="H24" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="10">
+        <v>340</v>
+      </c>
+      <c r="F25" s="23"/>
+      <c r="G25" s="7">
+        <v>16</v>
+      </c>
+      <c r="H25" s="14">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>